<commit_message>
real data descriptives table
</commit_message>
<xml_diff>
--- a/Config/realDataInfo.xlsx
+++ b/Config/realDataInfo.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zagre\Documents\probSimulator\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95661825-C2BD-405C-B05A-F4FC6132B1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C89F04E-07EA-4553-9483-224F07D9420D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3ABB0C20-75F1-43B9-B3BA-724C8F6A6404}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{3ABB0C20-75F1-43B9-B3BA-724C8F6A6404}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="config" sheetId="1" r:id="rId1"/>
+    <sheet name="descriptions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>neumayer</t>
   </si>
@@ -54,16 +55,67 @@
     <t>colnames</t>
   </si>
   <si>
-    <t>c()</t>
-  </si>
-  <si>
     <t>dataName</t>
   </si>
   <si>
-    <t>c("Multilateral Aid", "Log Population", "Log Pop Squared", "Log GDP", "Log Colony", "Log Distance", "Freedom", "Military Exp")</t>
-  </si>
-  <si>
     <t>distrList</t>
+  </si>
+  <si>
+    <t>Multilateral Aid</t>
+  </si>
+  <si>
+    <t>datadesc</t>
+  </si>
+  <si>
+    <t>Log Population</t>
+  </si>
+  <si>
+    <t>Log Pop Squared</t>
+  </si>
+  <si>
+    <t>Log GDP</t>
+  </si>
+  <si>
+    <t>Log Colony</t>
+  </si>
+  <si>
+    <t>Log Distance</t>
+  </si>
+  <si>
+    <t>Freedom</t>
+  </si>
+  <si>
+    <t>Military Exp</t>
+  </si>
+  <si>
+    <t>Log of population</t>
+  </si>
+  <si>
+    <t>Log of population^2</t>
+  </si>
+  <si>
+    <t>Log years of colonial experience</t>
+  </si>
+  <si>
+    <t>Log min. dist. to dev. world capital</t>
+  </si>
+  <si>
+    <t>Based on Freedom House</t>
+  </si>
+  <si>
+    <t>Military expenditures as share of budget</t>
+  </si>
+  <si>
+    <t>tmp</t>
+  </si>
+  <si>
+    <t>tmpDesc</t>
+  </si>
+  <si>
+    <t>Development Assistance (1995$)</t>
+  </si>
+  <si>
+    <t>Log of GDP (PPP) per capita (1995$)</t>
   </si>
 </sst>
 </file>
@@ -430,62 +482,404 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B9A0EB-9E3E-471C-9CB7-46D58B3D282A}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
+      <c r="C2" s="1" t="str">
+        <f ca="1">OFFSET(descriptions!$G$1,4,MATCH(config!$A2,descriptions!$G$1:$R$1,0)-1)</f>
+        <v>c("Multilateral Aid","Log Population","Log Pop Squared","Log GDP","Log Colony","Log Distance","Freedom","Military Exp")</v>
       </c>
       <c r="D2" t="str">
         <f>A2&amp;"Data"</f>
         <v>neumayerData</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="str">
+        <f ca="1">OFFSET(descriptions!$G$1,4,MATCH(config!$A2,descriptions!$G$1:$R$1,0))</f>
+        <v>c("Development Assistance (1995$)","Log of population","Log of population^2","Log of GDP (PPP) per capita (1995$)","Log years of colonial experience","Log min. dist. to dev. world capital","Based on Freedom House","Military expenditures as share of budget")</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
+      <c r="C3" s="1" t="str">
+        <f ca="1">OFFSET(descriptions!$G$1,4,MATCH(config!$A3,descriptions!$G$1:$R$1,0)-1)</f>
+        <v>c("tmp","tmp","tmp","tmp","tmp","tmp","tmp","tmp")</v>
       </c>
       <c r="D3" t="str">
         <f>A3&amp;"Data"</f>
         <v>drehJenData</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f ca="1">OFFSET(descriptions!$G$1,4,MATCH(config!$A3,descriptions!$G$1:$R$1,0))</f>
+        <v>c("tmpDesc","tmpDesc","tmpDesc","tmpDesc","tmpDesc","tmpDesc","tmpDesc","tmpDesc")</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CCC06AB-C021-4B40-B4DF-79944117204F}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G5" t="str">
+        <f>_xlfn.CONCAT("c(",G6:G13,")")</f>
+        <v>c("Multilateral Aid","Log Population","Log Pop Squared","Log GDP","Log Colony","Log Distance","Freedom","Military Exp")</v>
+      </c>
+      <c r="H5" t="str">
+        <f>_xlfn.CONCAT("c(",H6:H13,")")</f>
+        <v>c("Development Assistance (1995$)","Log of population","Log of population^2","Log of GDP (PPP) per capita (1995$)","Log years of colonial experience","Log min. dist. to dev. world capital","Based on Freedom House","Military expenditures as share of budget")</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" ref="I5:J5" si="0">_xlfn.CONCAT("c(",I6:I13,")")</f>
+        <v>c("tmp","tmp","tmp","tmp","tmp","tmp","tmp","tmp")</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>c("tmpDesc","tmpDesc","tmpDesc","tmpDesc","tmpDesc","tmpDesc","tmpDesc","tmpDesc")</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="str">
+        <f>""""&amp;A6&amp;""","</f>
+        <v>"Multilateral Aid",</v>
+      </c>
+      <c r="H6" t="str">
+        <f>""""&amp;B6&amp;""","</f>
+        <v>"Development Assistance (1995$)",</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" ref="I6:J12" si="1">""""&amp;C6&amp;""","</f>
+        <v>"tmp",</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="1"/>
+        <v>"tmpDesc",</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="str">
+        <f>""""&amp;A7&amp;""","</f>
+        <v>"Log Population",</v>
+      </c>
+      <c r="H7" t="str">
+        <f>""""&amp;B7&amp;""","</f>
+        <v>"Log of population",</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v>"tmp",</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="1"/>
+        <v>"tmpDesc",</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="str">
+        <f>""""&amp;A8&amp;""","</f>
+        <v>"Log Pop Squared",</v>
+      </c>
+      <c r="H8" t="str">
+        <f>""""&amp;B8&amp;""","</f>
+        <v>"Log of population^2",</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>"tmp",</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="1"/>
+        <v>"tmpDesc",</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="str">
+        <f>""""&amp;A9&amp;""","</f>
+        <v>"Log GDP",</v>
+      </c>
+      <c r="H9" t="str">
+        <f>""""&amp;B9&amp;""","</f>
+        <v>"Log of GDP (PPP) per capita (1995$)",</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v>"tmp",</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="1"/>
+        <v>"tmpDesc",</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="str">
+        <f>""""&amp;A10&amp;""","</f>
+        <v>"Log Colony",</v>
+      </c>
+      <c r="H10" t="str">
+        <f>""""&amp;B10&amp;""","</f>
+        <v>"Log years of colonial experience",</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="1"/>
+        <v>"tmp",</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="1"/>
+        <v>"tmpDesc",</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="str">
+        <f>""""&amp;A11&amp;""","</f>
+        <v>"Log Distance",</v>
+      </c>
+      <c r="H11" t="str">
+        <f>""""&amp;B11&amp;""","</f>
+        <v>"Log min. dist. to dev. world capital",</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="1"/>
+        <v>"tmp",</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="1"/>
+        <v>"tmpDesc",</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" t="str">
+        <f>""""&amp;A12&amp;""","</f>
+        <v>"Freedom",</v>
+      </c>
+      <c r="H12" t="str">
+        <f>""""&amp;B12&amp;""","</f>
+        <v>"Based on Freedom House",</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="1"/>
+        <v>"tmp",</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="1"/>
+        <v>"tmpDesc",</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="str">
+        <f>""""&amp;A13&amp;""""</f>
+        <v>"Military Exp"</v>
+      </c>
+      <c r="H13" t="str">
+        <f>""""&amp;B13&amp;""""</f>
+        <v>"Military expenditures as share of budget"</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" ref="I13:J13" si="2">""""&amp;C13&amp;""""</f>
+        <v>"tmp"</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="2"/>
+        <v>"tmpDesc"</v>
       </c>
     </row>
   </sheetData>

</xml_diff>